<commit_message>
KWR008 - report : update template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -75,6 +75,13 @@
     <definedName name="numExceedTime">★年間勤務表（1ヶ月）!$R$5</definedName>
     <definedName name="outputAgreementTime">★年間勤務表（1ヶ月）!$S$2</definedName>
     <definedName name="period">★年間勤務表（1ヶ月）!$A$1</definedName>
+    <definedName name="period1st">★年間勤務表（1ヶ月）!$S$5</definedName>
+    <definedName name="period2nd">★年間勤務表（1ヶ月）!$T$5</definedName>
+    <definedName name="period3rd">★年間勤務表（1ヶ月）!$U$5</definedName>
+    <definedName name="period4th">★年間勤務表（1ヶ月）!$V$5</definedName>
+    <definedName name="period5th">★年間勤務表（1ヶ月）!$W$5</definedName>
+    <definedName name="period6th">★年間勤務表（1ヶ月）!$X$5</definedName>
+    <definedName name="period7th">★年間勤務表（1ヶ月）!$Y$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">★年間勤務表（1ヶ月）!$1:$3</definedName>
     <definedName name="sum">★年間勤務表（1ヶ月）!$Q$5</definedName>
     <definedName name="workplace">★年間勤務表（1ヶ月）!$A$4</definedName>
@@ -854,6 +861,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -886,15 +902,6 @@
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1286,11 +1293,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="A1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -1342,8 +1349,8 @@
       <c r="Z2" s="38"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="37"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -1374,12 +1381,12 @@
       <c r="Z3" s="38"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="35"/>
       <c r="H4" s="35"/>
       <c r="I4" s="22"/>
@@ -1401,35 +1408,35 @@
       <c r="Y4" s="18"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="52"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="23"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1455,8 +1462,8 @@
       <c r="Y6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="24"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>

</xml_diff>

<commit_message>
KWR008 A: CR No405
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\NITTSU\UniversalK2\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NITTSU\PJ\KWR008\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,65 +28,64 @@
     <definedName name="_Sort" hidden="1">#REF!</definedName>
     <definedName name="abc" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="abc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
-    <definedName name="average">★年間勤務表（1ヶ月）!$P$5</definedName>
+    <definedName name="average">'★年間勤務表（1ヶ月）'!$P$5</definedName>
     <definedName name="def" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="def" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
-    <definedName name="empInfo">★年間勤務表（1ヶ月）!$A$5:$B$14</definedName>
-    <definedName name="empInfoLabel">★年間勤務表（1ヶ月）!$A$3</definedName>
-    <definedName name="employeeRange">★年間勤務表（1ヶ月）!$A$5:$Y$14</definedName>
-    <definedName name="employmentName">★年間勤務表（1ヶ月）!$A$6</definedName>
-    <definedName name="empName">★年間勤務表（1ヶ月）!$A$5</definedName>
-    <definedName name="item">★年間勤務表（1ヶ月）!$C$5</definedName>
-    <definedName name="jobTitle">★年間勤務表（1ヶ月）!$A$7</definedName>
+    <definedName name="empInfoLabel">'★年間勤務表（1ヶ月）'!$A$3</definedName>
+    <definedName name="employeeRange">'★年間勤務表（1ヶ月）'!$A$5:$Z$14</definedName>
+    <definedName name="employmentName">'★年間勤務表（1ヶ月）'!$A$6</definedName>
+    <definedName name="empName">'★年間勤務表（1ヶ月）'!$A$5</definedName>
+    <definedName name="item">'★年間勤務表（1ヶ月）'!$C$5</definedName>
+    <definedName name="jobTitle">'★年間勤務表（1ヶ月）'!$A$7</definedName>
     <definedName name="kkkk" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="kkkk" hidden="1">#REF!</definedName>
-    <definedName name="month10th">★年間勤務表（1ヶ月）!$M$5</definedName>
-    <definedName name="month10thLabel">★年間勤務表（1ヶ月）!$M$3</definedName>
-    <definedName name="month11th">★年間勤務表（1ヶ月）!$N$5</definedName>
-    <definedName name="month11thLabel">★年間勤務表（1ヶ月）!$N$3</definedName>
-    <definedName name="month12th">★年間勤務表（1ヶ月）!$O$5</definedName>
-    <definedName name="month12thLabel">★年間勤務表（1ヶ月）!$O$3</definedName>
-    <definedName name="month1st">★年間勤務表（1ヶ月）!$D$5</definedName>
-    <definedName name="month1stLabel">★年間勤務表（1ヶ月）!$D$3</definedName>
-    <definedName name="month2nd">★年間勤務表（1ヶ月）!$E$5</definedName>
-    <definedName name="month2ndLabel">★年間勤務表（1ヶ月）!$E$3</definedName>
-    <definedName name="month3rd">★年間勤務表（1ヶ月）!$F$5</definedName>
-    <definedName name="month3rdLabel">★年間勤務表（1ヶ月）!$F$3</definedName>
-    <definedName name="month4th">★年間勤務表（1ヶ月）!$G$5</definedName>
-    <definedName name="month4thLabel">★年間勤務表（1ヶ月）!$G$3</definedName>
-    <definedName name="month5th">★年間勤務表（1ヶ月）!$H$5</definedName>
-    <definedName name="month5thLabel">★年間勤務表（1ヶ月）!$H$3</definedName>
-    <definedName name="month6th">★年間勤務表（1ヶ月）!$I$5</definedName>
-    <definedName name="month6thLabel">★年間勤務表（1ヶ月）!$I$3</definedName>
-    <definedName name="month7th">★年間勤務表（1ヶ月）!$J$5</definedName>
-    <definedName name="month7thLabel">★年間勤務表（1ヶ月）!$J$3</definedName>
-    <definedName name="month8th">★年間勤務表（1ヶ月）!$K$5</definedName>
-    <definedName name="month8thLabel">★年間勤務表（1ヶ月）!$K$3</definedName>
-    <definedName name="month9th">★年間勤務表（1ヶ月）!$L$5</definedName>
-    <definedName name="month9thLabel">★年間勤務表（1ヶ月）!$L$3</definedName>
-    <definedName name="monthPeriod6Range">★年間勤務表（1ヶ月）!$X$2:$X$3</definedName>
-    <definedName name="monthPeriodLabel1">★年間勤務表（1ヶ月）!$S$3</definedName>
-    <definedName name="monthPeriodLabel2">★年間勤務表（1ヶ月）!$T$3</definedName>
-    <definedName name="monthPeriodLabel3">★年間勤務表（1ヶ月）!$U$3</definedName>
-    <definedName name="monthPeriodLabel4">★年間勤務表（1ヶ月）!$V$3</definedName>
-    <definedName name="monthPeriodLabel5">★年間勤務表（1ヶ月）!$W$3</definedName>
-    <definedName name="monthPeriodLabel6">★年間勤務表（1ヶ月）!$X$3</definedName>
-    <definedName name="monthPeriodLabel7">★年間勤務表（1ヶ月）!$Y$3</definedName>
-    <definedName name="numExceedTime">★年間勤務表（1ヶ月）!$R$5</definedName>
-    <definedName name="outputAgreementTime">★年間勤務表（1ヶ月）!$S$2</definedName>
-    <definedName name="period">★年間勤務表（1ヶ月）!$A$1</definedName>
-    <definedName name="period1st">★年間勤務表（1ヶ月）!$S$5</definedName>
-    <definedName name="period2nd">★年間勤務表（1ヶ月）!$T$5</definedName>
-    <definedName name="period3rd">★年間勤務表（1ヶ月）!$U$5</definedName>
-    <definedName name="period4th">★年間勤務表（1ヶ月）!$V$5</definedName>
-    <definedName name="period5th">★年間勤務表（1ヶ月）!$W$5</definedName>
-    <definedName name="period6th">★年間勤務表（1ヶ月）!$X$5</definedName>
-    <definedName name="period7th">★年間勤務表（1ヶ月）!$Y$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">★年間勤務表（1ヶ月）!$1:$3</definedName>
-    <definedName name="sum">★年間勤務表（1ヶ月）!$Q$5</definedName>
-    <definedName name="workplace">★年間勤務表（1ヶ月）!$A$4</definedName>
-    <definedName name="workplaceRange">★年間勤務表（1ヶ月）!$A$4:$Y$14</definedName>
-    <definedName name="workplaceRow">★年間勤務表（1ヶ月）!$A$4:$Y$4</definedName>
+    <definedName name="month10th">'★年間勤務表（1ヶ月）'!$M$5</definedName>
+    <definedName name="month10thLabel">'★年間勤務表（1ヶ月）'!$M$3</definedName>
+    <definedName name="month11th">'★年間勤務表（1ヶ月）'!$N$5</definedName>
+    <definedName name="month11thLabel">'★年間勤務表（1ヶ月）'!$N$3</definedName>
+    <definedName name="month12th">'★年間勤務表（1ヶ月）'!$O$5</definedName>
+    <definedName name="month12thLabel">'★年間勤務表（1ヶ月）'!$O$3</definedName>
+    <definedName name="month1st">'★年間勤務表（1ヶ月）'!$D$5</definedName>
+    <definedName name="month1stLabel">'★年間勤務表（1ヶ月）'!$D$3</definedName>
+    <definedName name="month2nd">'★年間勤務表（1ヶ月）'!$E$5</definedName>
+    <definedName name="month2ndLabel">'★年間勤務表（1ヶ月）'!$E$3</definedName>
+    <definedName name="month3rd">'★年間勤務表（1ヶ月）'!$F$5</definedName>
+    <definedName name="month3rdLabel">'★年間勤務表（1ヶ月）'!$F$3</definedName>
+    <definedName name="month4th">'★年間勤務表（1ヶ月）'!$G$5</definedName>
+    <definedName name="month4thLabel">'★年間勤務表（1ヶ月）'!$G$3</definedName>
+    <definedName name="month5th">'★年間勤務表（1ヶ月）'!$H$5</definedName>
+    <definedName name="month5thLabel">'★年間勤務表（1ヶ月）'!$H$3</definedName>
+    <definedName name="month6th">'★年間勤務表（1ヶ月）'!$I$5</definedName>
+    <definedName name="month6thLabel">'★年間勤務表（1ヶ月）'!$I$3</definedName>
+    <definedName name="month7th">'★年間勤務表（1ヶ月）'!$J$5</definedName>
+    <definedName name="month7thLabel">'★年間勤務表（1ヶ月）'!$J$3</definedName>
+    <definedName name="month8th">'★年間勤務表（1ヶ月）'!$K$5</definedName>
+    <definedName name="month8thLabel">'★年間勤務表（1ヶ月）'!$K$3</definedName>
+    <definedName name="month9th">'★年間勤務表（1ヶ月）'!$L$5</definedName>
+    <definedName name="month9thLabel">'★年間勤務表（1ヶ月）'!$L$3</definedName>
+    <definedName name="monthPeriod6Range">'★年間勤務表（1ヶ月）'!$Y$2:$Y$3</definedName>
+    <definedName name="monthPeriodLabel1">'★年間勤務表（1ヶ月）'!$T$3</definedName>
+    <definedName name="monthPeriodLabel2">'★年間勤務表（1ヶ月）'!$U$3</definedName>
+    <definedName name="monthPeriodLabel3">'★年間勤務表（1ヶ月）'!$V$3</definedName>
+    <definedName name="monthPeriodLabel4">'★年間勤務表（1ヶ月）'!$W$3</definedName>
+    <definedName name="monthPeriodLabel5">'★年間勤務表（1ヶ月）'!$X$3</definedName>
+    <definedName name="monthPeriodLabel6">'★年間勤務表（1ヶ月）'!$Y$3</definedName>
+    <definedName name="monthPeriodLabel7">'★年間勤務表（1ヶ月）'!$Z$3</definedName>
+    <definedName name="numExceedTime">'★年間勤務表（1ヶ月）'!$R$5</definedName>
+    <definedName name="numExceedTime1">'★年間勤務表（1ヶ月）'!$R$5</definedName>
+    <definedName name="numRemainingTime">'★年間勤務表（1ヶ月）'!$S$5</definedName>
+    <definedName name="outputAgreementTime">'★年間勤務表（1ヶ月）'!$T$2</definedName>
+    <definedName name="period">'★年間勤務表（1ヶ月）'!$A$1</definedName>
+    <definedName name="period1st">'★年間勤務表（1ヶ月）'!$T$5</definedName>
+    <definedName name="period2nd">'★年間勤務表（1ヶ月）'!$U$5</definedName>
+    <definedName name="period3rd">'★年間勤務表（1ヶ月）'!$V$5</definedName>
+    <definedName name="period4th">'★年間勤務表（1ヶ月）'!$W$5</definedName>
+    <definedName name="period5th">'★年間勤務表（1ヶ月）'!$X$5</definedName>
+    <definedName name="period6th">'★年間勤務表（1ヶ月）'!$Y$5</definedName>
+    <definedName name="period7th">'★年間勤務表（1ヶ月）'!$Z$5</definedName>
+    <definedName name="sum">'★年間勤務表（1ヶ月）'!$Q$5</definedName>
+    <definedName name="workplace">'★年間勤務表（1ヶ月）'!$A$4</definedName>
+    <definedName name="workplaceRange">'★年間勤務表（1ヶ月）'!$A$4:$Z$14</definedName>
     <definedName name="wrn.MIND." localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.MIND." hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="あああ" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -101,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>年間</t>
     <phoneticPr fontId="3"/>
@@ -124,11 +123,15 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
+    <t>月</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
     <t>平均</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>月</t>
+    <t>残数</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -137,13 +140,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
-    <numFmt numFmtId="170" formatCode="0&quot;回&quot;;;;@"/>
+    <numFmt numFmtId="176" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="0.000%"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="181" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
+    <numFmt numFmtId="182" formatCode="0&quot;回&quot;;;;@"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -293,7 +296,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -301,7 +304,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -626,9 +629,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -643,7 +646,7 @@
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" applyProtection="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="181" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="right"/>
@@ -658,8 +661,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -871,7 +874,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1278,7 +1281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -1286,17 +1289,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="8.28515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="7.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
     <col min="4" max="14" width="5.42578125" style="1" customWidth="1"/>
     <col min="15" max="17" width="5.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" style="2" customWidth="1"/>
-    <col min="19" max="24" width="5.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="5.42578125" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="3.140625" style="2"/>
+    <col min="18" max="19" width="3.7109375" style="2" customWidth="1"/>
+    <col min="20" max="25" width="5.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="3.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="44"/>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -1311,14 +1314,14 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
-      <c r="S1" s="4"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1">
+      <c r="Y1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" ht="15" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="8"/>
@@ -1335,7 +1338,7 @@
       <c r="N2" s="33"/>
       <c r="O2" s="33"/>
       <c r="P2" s="32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="21" t="s">
         <v>0</v>
@@ -1343,16 +1346,19 @@
       <c r="R2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="14"/>
+      <c r="S2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="21"/>
       <c r="U2" s="14"/>
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
       <c r="X2" s="14"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="38"/>
-    </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="38"/>
+    </row>
+    <row r="3" spans="1:27" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="52"/>
       <c r="B3" s="52"/>
       <c r="C3" s="37"/>
@@ -1369,22 +1375,25 @@
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
       <c r="P3" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="16"/>
+      <c r="S3" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="T3" s="16"/>
       <c r="U3" s="16"/>
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
       <c r="X3" s="16"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="38"/>
-    </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="38"/>
+    </row>
+    <row r="4" spans="1:27" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="46"/>
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
@@ -1403,15 +1412,16 @@
       <c r="P4" s="19"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="19"/>
-      <c r="S4" s="20"/>
+      <c r="S4" s="19"/>
       <c r="T4" s="20"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="22"/>
       <c r="W4" s="20"/>
       <c r="X4" s="20"/>
-      <c r="Y4" s="18"/>
-    </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1">
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="18"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" customHeight="1">
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
       <c r="C5" s="40"/>
@@ -1430,15 +1440,16 @@
       <c r="P5" s="41"/>
       <c r="Q5" s="42"/>
       <c r="R5" s="43"/>
-      <c r="S5" s="41"/>
+      <c r="S5" s="43"/>
       <c r="T5" s="41"/>
       <c r="U5" s="41"/>
       <c r="V5" s="41"/>
       <c r="W5" s="41"/>
       <c r="X5" s="41"/>
       <c r="Y5" s="41"/>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1">
+      <c r="Z5" s="41"/>
+    </row>
+    <row r="6" spans="1:27" ht="15" customHeight="1">
       <c r="A6" s="49"/>
       <c r="B6" s="50"/>
       <c r="C6" s="23"/>
@@ -1464,8 +1475,9 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1">
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" ht="15" customHeight="1">
       <c r="A7" s="49"/>
       <c r="B7" s="51"/>
       <c r="C7" s="24"/>
@@ -1491,8 +1503,9 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
+      <c r="Z7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="15" customHeight="1">
       <c r="A8" s="29"/>
       <c r="B8" s="30"/>
       <c r="C8" s="25"/>
@@ -1518,8 +1531,9 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1">
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" ht="15" customHeight="1">
       <c r="A9" s="29"/>
       <c r="B9" s="30"/>
       <c r="C9" s="26"/>
@@ -1545,8 +1559,9 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1">
+      <c r="Z9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" ht="15" customHeight="1">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="25"/>
@@ -1572,8 +1587,9 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1">
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" ht="15" customHeight="1">
       <c r="A11" s="29"/>
       <c r="B11" s="30"/>
       <c r="C11" s="26"/>
@@ -1599,8 +1615,9 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1">
+      <c r="Z11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" ht="15" customHeight="1">
       <c r="A12" s="29"/>
       <c r="B12" s="30"/>
       <c r="C12" s="25"/>
@@ -1626,8 +1643,9 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1">
+      <c r="Z12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" ht="15" customHeight="1">
       <c r="A13" s="29"/>
       <c r="B13" s="30"/>
       <c r="C13" s="26"/>
@@ -1653,8 +1671,9 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
+      <c r="Z13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" ht="15" customHeight="1" thickBot="1">
       <c r="A14" s="28"/>
       <c r="B14" s="31"/>
       <c r="C14" s="27"/>
@@ -1680,11 +1699,12 @@
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
-    </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1">
+      <c r="Z14" s="7"/>
+    </row>
+    <row r="15" spans="1:27" ht="15" customHeight="1">
       <c r="E15" s="39"/>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1">
+    <row r="16" spans="1:27" ht="15" customHeight="1">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -1710,8 +1730,9 @@
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
       <c r="Y16" s="36"/>
-    </row>
-    <row r="17" spans="1:25" ht="15" customHeight="1">
+      <c r="Z16" s="36"/>
+    </row>
+    <row r="17" spans="1:26" ht="15" customHeight="1">
       <c r="A17" s="36"/>
       <c r="B17" s="36"/>
       <c r="C17" s="36"/>
@@ -1737,8 +1758,9 @@
       <c r="W17" s="36"/>
       <c r="X17" s="36"/>
       <c r="Y17" s="36"/>
-    </row>
-    <row r="18" spans="1:25" ht="15" customHeight="1">
+      <c r="Z17" s="36"/>
+    </row>
+    <row r="18" spans="1:26" ht="15" customHeight="1">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -1764,8 +1786,9 @@
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
       <c r="Y18" s="36"/>
-    </row>
-    <row r="19" spans="1:25" ht="15" customHeight="1">
+      <c r="Z18" s="36"/>
+    </row>
+    <row r="19" spans="1:26" ht="15" customHeight="1">
       <c r="A19" s="36"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
@@ -1791,8 +1814,9 @@
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
       <c r="Y19" s="36"/>
-    </row>
-    <row r="20" spans="1:25" ht="15" customHeight="1">
+      <c r="Z19" s="36"/>
+    </row>
+    <row r="20" spans="1:26" ht="15" customHeight="1">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -1818,8 +1842,9 @@
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
       <c r="Y20" s="36"/>
-    </row>
-    <row r="21" spans="1:25" ht="15" customHeight="1">
+      <c r="Z20" s="36"/>
+    </row>
+    <row r="21" spans="1:26" ht="15" customHeight="1">
       <c r="A21" s="36"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -1845,8 +1870,9 @@
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
       <c r="Y21" s="36"/>
-    </row>
-    <row r="22" spans="1:25" ht="15" customHeight="1">
+      <c r="Z21" s="36"/>
+    </row>
+    <row r="22" spans="1:26" ht="15" customHeight="1">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -1872,8 +1898,9 @@
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
       <c r="Y22" s="36"/>
-    </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1">
+      <c r="Z22" s="36"/>
+    </row>
+    <row r="23" spans="1:26" ht="15" customHeight="1">
       <c r="A23" s="36"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -1899,8 +1926,9 @@
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
       <c r="Y23" s="36"/>
-    </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1">
+      <c r="Z23" s="36"/>
+    </row>
+    <row r="24" spans="1:26" ht="15" customHeight="1">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -1926,8 +1954,9 @@
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
       <c r="Y24" s="36"/>
-    </row>
-    <row r="25" spans="1:25" ht="15" customHeight="1">
+      <c r="Z24" s="36"/>
+    </row>
+    <row r="25" spans="1:26" ht="15" customHeight="1">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -1953,6 +1982,7 @@
       <c r="W25" s="36"/>
       <c r="X25" s="36"/>
       <c r="Y25" s="36"/>
+      <c r="Z25" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
KWR008: update cột remaining
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -139,14 +139,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="176" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
     <numFmt numFmtId="177" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="0.000%"/>
     <numFmt numFmtId="180" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="181" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
-    <numFmt numFmtId="182" formatCode="0&quot;回&quot;;;;@"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -744,7 +743,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -872,9 +871,6 @@
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1300,11 +1296,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="A1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -1359,8 +1355,8 @@
       <c r="AA2" s="38"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="37"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -1394,12 +1390,12 @@
       <c r="AA3" s="38"/>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="35"/>
       <c r="H4" s="35"/>
       <c r="I4" s="22"/>
@@ -1422,8 +1418,8 @@
       <c r="Z4" s="18"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="40"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
@@ -1439,8 +1435,8 @@
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
       <c r="Q5" s="42"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
       <c r="T5" s="41"/>
       <c r="U5" s="41"/>
       <c r="V5" s="41"/>
@@ -1450,8 +1446,8 @@
       <c r="Z5" s="41"/>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="23"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1478,8 +1474,8 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="49"/>
-      <c r="B7" s="51"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="24"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>

</xml_diff>

<commit_message>
set border thick for first value of employee range
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -919,6 +919,9 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,9 +933,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1346,9 +1346,9 @@
       <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="12"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -1382,9 +1382,9 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -1416,31 +1416,31 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="43"/>

</xml_diff>

<commit_message>
Fix bug KWR008 #119594
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\UniversalK_clone\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878F00F6-B732-4319-B2B1-3279B66C9490}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE153A0-C2F5-4F74-A846-F08CB88D8E93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1343,10 +1343,10 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="P18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.109375" defaultRowHeight="14.4" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="8.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
@@ -1358,7 +1358,7 @@
     <col min="26" max="16384" width="3.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:26" ht="14.4" customHeight="1" thickBot="1">
       <c r="A1" s="38"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -1380,7 +1380,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1">
+    <row r="2" spans="1:26" ht="14.4" customHeight="1">
       <c r="A2" s="46"/>
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
@@ -1416,7 +1416,7 @@
       <c r="Y2" s="37"/>
       <c r="Z2" s="9"/>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:26" ht="14.4" customHeight="1" thickBot="1">
       <c r="A3" s="48"/>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
@@ -1450,7 +1450,7 @@
       <c r="Y3" s="31"/>
       <c r="Z3" s="9"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:26" ht="14.4" customHeight="1" thickBot="1">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
@@ -1477,7 +1477,7 @@
       <c r="X4" s="45"/>
       <c r="Y4" s="45"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1">
+    <row r="5" spans="1:26" ht="14.4" customHeight="1">
       <c r="A5" s="43"/>
       <c r="B5" s="44"/>
       <c r="C5" s="24"/>
@@ -1504,7 +1504,7 @@
       <c r="X5" s="25"/>
       <c r="Y5" s="27"/>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1">
+    <row r="6" spans="1:26" ht="14.4" customHeight="1">
       <c r="A6" s="40"/>
       <c r="B6" s="41"/>
       <c r="C6" s="14"/>
@@ -1531,7 +1531,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="22"/>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1">
+    <row r="7" spans="1:26" ht="14.4" customHeight="1">
       <c r="A7" s="40"/>
       <c r="B7" s="42"/>
       <c r="C7" s="17"/>
@@ -1558,7 +1558,7 @@
       <c r="X7" s="18"/>
       <c r="Y7" s="23"/>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
+    <row r="8" spans="1:26" ht="14.4" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="20"/>
@@ -1585,7 +1585,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="22"/>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1">
+    <row r="9" spans="1:26" ht="14.4" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="21"/>
@@ -1612,7 +1612,7 @@
       <c r="X9" s="18"/>
       <c r="Y9" s="23"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1">
+    <row r="10" spans="1:26" ht="14.4" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="20"/>
@@ -1639,7 +1639,7 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="22"/>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1">
+    <row r="11" spans="1:26" ht="14.4" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="21"/>
@@ -1666,7 +1666,7 @@
       <c r="X11" s="18"/>
       <c r="Y11" s="23"/>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1">
+    <row r="12" spans="1:26" ht="14.4" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="20"/>
@@ -1693,7 +1693,7 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="22"/>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1">
+    <row r="13" spans="1:26" ht="14.4" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="21"/>
@@ -1720,7 +1720,7 @@
       <c r="X13" s="18"/>
       <c r="Y13" s="23"/>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1">
+    <row r="14" spans="1:26" ht="14.4" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="20"/>
@@ -1747,7 +1747,7 @@
       <c r="X14" s="15"/>
       <c r="Y14" s="22"/>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1">
+    <row r="15" spans="1:26" ht="14.4" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="33"/>
@@ -1774,10 +1774,10 @@
       <c r="X15" s="34"/>
       <c r="Y15" s="35"/>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1">
+    <row r="16" spans="1:26" ht="14.4" customHeight="1">
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:25" ht="15" customHeight="1">
+    <row r="17" spans="1:25" ht="14.4" customHeight="1">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1804,7 +1804,7 @@
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" ht="15" customHeight="1">
+    <row r="18" spans="1:25" ht="14.4" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1831,7 +1831,7 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25" ht="15" customHeight="1">
+    <row r="19" spans="1:25" ht="14.4" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1858,7 +1858,7 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" ht="15" customHeight="1">
+    <row r="20" spans="1:25" ht="14.4" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1885,7 +1885,7 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" spans="1:25" ht="15" customHeight="1">
+    <row r="21" spans="1:25" ht="14.4" customHeight="1">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1912,7 +1912,7 @@
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
     </row>
-    <row r="22" spans="1:25" ht="15" customHeight="1">
+    <row r="22" spans="1:25" ht="14.4" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1939,7 +1939,7 @@
       <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1">
+    <row r="23" spans="1:25" ht="14.4" customHeight="1">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1966,7 +1966,7 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1">
+    <row r="24" spans="1:25" ht="14.4" customHeight="1">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1993,7 +1993,7 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" ht="15" customHeight="1">
+    <row r="25" spans="1:25" ht="14.4" customHeight="1">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2020,7 +2020,7 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1">
+    <row r="26" spans="1:25" ht="14.4" customHeight="1">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>

</xml_diff>

<commit_message>
Fix bug KWR008 #119799
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\UniversalK_clone\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE153A0-C2F5-4F74-A846-F08CB88D8E93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF12C05-E666-4EB0-98CE-169DAA3254B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,7 +784,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -923,17 +923,23 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1343,7 +1349,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="P18" sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.109375" defaultRowHeight="14.4" customHeight="1"/>
@@ -1381,9 +1387,9 @@
       <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="14.4" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="12"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -1417,9 +1423,9 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="14.4" customHeight="1" thickBot="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>

</xml_diff>